<commit_message>
updated templates and change docs
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/15-BulkUploadMonthlyRequirement.xlsx
+++ b/documents/templates/bulk-upload/15-BulkUploadMonthlyRequirement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C245FA84-3B28-0E4F-A15C-2F3A894F62FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE198E98-AC27-8041-8BE1-FF9A6729A9F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{6BC27182-73A8-D94B-97E4-67DF06DD5638}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{6BC27182-73A8-D94B-97E4-67DF06DD5638}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Part Number</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Schedule Name</t>
-  </si>
-  <si>
-    <t>DL01 Shortage</t>
   </si>
   <si>
     <t>Description</t>
@@ -504,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00918543-CCCC-1A4B-991F-874C25238D88}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,8 +510,10 @@
     <col min="1" max="1" width="10.5" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,25 +531,25 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -561,19 +560,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>319013083002</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2" s="4">
         <v>1348</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -583,30 +582,28 @@
       <c r="B3" s="3">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="2">
         <v>319021083065</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="5">
         <v>509</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>